<commit_message>
Typo correction in test util
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -1,25 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahilsha\Documents\workspace-sts\HairAdvisor\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="3225" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="3225"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
-    <sheet name="output" sheetId="5" r:id="rId5"/>
+    <sheet name="output" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -28,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Testcase1</t>
   </si>
@@ -57,24 +50,36 @@
     <t>ff</t>
   </si>
   <si>
+    <t>jj</t>
+  </si>
+  <si>
+    <t>dad</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
     <t>keval - Google Search</t>
   </si>
   <si>
+    <t>2.0</t>
+  </si>
+  <si>
     <t>rahil - Google Search</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>2.0</t>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>dad - Google Search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,7 +219,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,24 +403,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -426,7 +431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -437,7 +442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -448,12 +453,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -464,7 +469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -475,7 +480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -484,6 +489,17 @@
       </c>
       <c r="C9" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -492,254 +508,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
     <col min="5" max="6" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
+    <row r="2">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
+    <row r="3">
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>